<commit_message>
Fix Total row in Competitions with dosage
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Работа</t>
   </si>
@@ -44,10 +44,13 @@
     <t>Сортировку сделать внутри выборки также по убыванию/возрастанию с возможностью выбора - отдельно</t>
   </si>
   <si>
-    <t>В анализе упаковок и анализе цены добавить sku ( с функцие select в настройках)</t>
+    <t>В паспортах указать ДОли компании в общих закупках (продажах)</t>
   </si>
   <si>
-    <t>В паспортах указать ДОли компании в общих закупках (продажах)</t>
+    <t>В анализе упаковок и анализе цены добавить sku ( с функцией select в настройках)</t>
+  </si>
+  <si>
+    <t>В Конкурентном анализе (ЛПУ и Рынки) добавить sku ( с функцией select в настройках)</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +457,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -469,19 +472,23 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>43506</v>
+      </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add LOGA-7 scripts for market create
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Работа</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>В Конкурентном анализе (ЛПУ и Рынки) добавить sku ( с функцией select в настройках)</t>
+  </si>
+  <si>
+    <t>Анализ, формированеи рынков для организации ЛИГА-7</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных</t>
   </si>
 </sst>
 </file>
@@ -407,7 +413,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,36 +505,48 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>43512</v>
+      </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>43510</v>
+      </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43512</v>
+      </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add chosen for fk fields
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Работа</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Сортировку сделать внутри выборки также по убыванию/возрастанию с возможностью выбора - отдельно</t>
   </si>
   <si>
-    <t>В паспортах указать ДОли компании в общих закупках (продажах)</t>
-  </si>
-  <si>
     <t>В анализе упаковок и анализе цены добавить sku ( с функцией select в настройках)</t>
   </si>
   <si>
@@ -56,10 +53,22 @@
     <t>Анализ, формированеи рынков для организации ЛИГА-7</t>
   </si>
   <si>
-    <t>Работа по созданию функционала загрузки данных</t>
-  </si>
-  <si>
     <t>ИТОГО</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (DatePicker, Валидация Int, Float, date)</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (Разработка строки ввода с выбором элемента сравнения)</t>
+  </si>
+  <si>
+    <t>Доработка Side-Button открывающей фильтры</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (Разработка каркаса приложения, структуры филтров)</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (Разработка, концепции, внешнего вида)</t>
   </si>
 </sst>
 </file>
@@ -415,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +475,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -481,7 +490,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>1.5</v>
@@ -496,41 +505,43 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>43512</v>
+      </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3">
-        <v>43512</v>
+        <v>43510</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="3">
-        <v>43510</v>
+        <v>43512</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
@@ -539,54 +550,62 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="3">
-        <v>43512</v>
+        <v>43513</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>43514</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>43516</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-      <c r="C11" s="3">
-        <v>43513</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
       <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>43517</v>
+      </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -844,11 +863,11 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D38">
         <f>SUM(D4:D37)</f>
-        <v>15500</v>
+        <v>22500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change fint-suze for select 10px to 12px
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Работа</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Работа по созданию функционала загрузки данных (chosen для fk полей)</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (замена chosen на select2)</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +447,7 @@
         <v>2</v>
       </c>
       <c r="B1">
-        <v>1000</v>
+        <v>800</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -473,7 +476,7 @@
       </c>
       <c r="D4" s="1">
         <f>B4*$B$1</f>
-        <v>2000</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -488,7 +491,7 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" ref="D5:D36" si="0">B5*$B$1</f>
-        <v>4000</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -503,7 +506,7 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -518,7 +521,7 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>800</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -533,7 +536,7 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -548,7 +551,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -563,7 +566,7 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -578,7 +581,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>800</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -593,7 +596,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -608,7 +611,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,18 +626,22 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>43521</v>
+      </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -874,7 +881,7 @@
       </c>
       <c r="D38">
         <f>SUM(D4:D37)</f>
-        <v>26500</v>
+        <v>22800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create add buttons for new filter input
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Работа</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Работа по созданию функционала загрузки данных (замена chosen на select2)</t>
+  </si>
+  <si>
+    <t>Создание скрипта для копирования сотрудников из одной компании в другую с привязкой е ЛПУ и Регионам</t>
   </si>
 </sst>
 </file>
@@ -431,7 +434,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,14 +648,18 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>43522</v>
+      </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -881,7 +888,7 @@
       </c>
       <c r="D38">
         <f>SUM(D4:D37)</f>
-        <v>22800</v>
+        <v>23200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Construct filters query for load data
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Работа</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Создание скрипта для копирования сотрудников из одной компании в другую с привязкой е ЛПУ и Регионам</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных</t>
   </si>
 </sst>
 </file>
@@ -434,7 +437,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,36 +666,48 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>43549</v>
+      </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C18" s="3">
+        <v>43550</v>
+      </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>43551</v>
+      </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -888,7 +903,7 @@
       </c>
       <c r="D38">
         <f>SUM(D4:D37)</f>
-        <v>23200</v>
+        <v>28000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create download with list fields
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Работа</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Работа по созданию функционала загрузки данных</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (Добавление офтальмологии)</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,14 +714,18 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>43552</v>
+      </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>800</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -903,7 +910,7 @@
       </c>
       <c r="D38">
         <f>SUM(D4:D37)</f>
-        <v>28000</v>
+        <v>28800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Group set/reset buttons in dataloader page
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Работа</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Работа по созданию функционала загрузки данных (Добавление офтальмологии)</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (Первый альфа вариант)</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,14 +732,18 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C21" s="3">
+        <v>43555</v>
+      </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -910,7 +917,7 @@
       </c>
       <c r="D38">
         <f>SUM(D4:D37)</f>
-        <v>28800</v>
+        <v>31200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add operation: Clear Filter; Save Filter; Table Filter
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Работа</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Работа по созданию функционала загрузки данных (Первый альфа вариант)</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (Групповые кнопки полей/фильтров)</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,14 +750,18 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C22" s="3">
+        <v>43566</v>
+      </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -917,7 +924,7 @@
       </c>
       <c r="D38">
         <f>SUM(D4:D37)</f>
-        <v>31200</v>
+        <v>32800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Async ajax for save filter
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Работа</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Работа по созданию функционала загрузки данных (Групповые кнопки полей/фильтров)</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (Запись фильтров)</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (Очистка фильтров, Таблица фильтров, модель хранения)</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,25 +771,33 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C23" s="3">
+        <v>43569</v>
+      </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C24" s="3">
+        <v>43570</v>
+      </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>800</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -924,7 +938,7 @@
       </c>
       <c r="D38">
         <f>SUM(D4:D37)</f>
-        <v>32800</v>
+        <v>35200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create button 'Save and Load'. Formatting datetime in filters table
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Работа</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Работа по созданию функционала загрузки данных (Загрузка фильтров, Настройка Celery+Redis)</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (Отложенная загрузка данных с Celery)</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,14 +876,18 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B29" s="1">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C29" s="3">
+        <v>43579</v>
+      </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -966,7 +973,7 @@
       </c>
       <c r="D38">
         <f>SUM(D4:D37)</f>
-        <v>42400</v>
+        <v>44800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add FO, Budgets and Winner FK
</commit_message>
<xml_diff>
--- a/DOC/Timeline/TimeLine.xlsx
+++ b/DOC/Timeline/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Работа</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Работа по созданию функционала загрузки данных (Отложенная загрузка данных с Celery)</t>
+  </si>
+  <si>
+    <t>Работа по созданию функционала загрузки данных (Функция SaveAndLoad, Формат даты и времени, Изменения алгоритма для ForeignKey, Настройка нескольких полей включая FK)</t>
   </si>
 </sst>
 </file>
@@ -466,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,14 +894,18 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C30" s="3">
+        <v>43585</v>
+      </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,7 +980,7 @@
       </c>
       <c r="D38">
         <f>SUM(D4:D37)</f>
-        <v>44800</v>
+        <v>47200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>